<commit_message>
refining some parameters, got within 10% of hieus data
</commit_message>
<xml_diff>
--- a/ptx_200_7d.xlsx
+++ b/ptx_200_7d.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430D9CA9-1A2B-4412-B7B1-CD862D0F4329}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5288BDE-412D-415B-B582-8CC4996473E1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11292" windowHeight="9492" xr2:uid="{EB34CEDC-EA5B-42AF-AF24-E312CA63D926}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
   <si>
     <t>Group</t>
   </si>
@@ -305,18 +305,6 @@
     <t>hieu ncv</t>
   </si>
   <si>
-    <t>my ncv median</t>
-  </si>
-  <si>
-    <t>hieu ncv median</t>
-  </si>
-  <si>
-    <t>my ncv average</t>
-  </si>
-  <si>
-    <t>hieu ncv average</t>
-  </si>
-  <si>
     <t>CONTROLS</t>
   </si>
   <si>
@@ -330,6 +318,9 @@
   </si>
   <si>
     <t>hieu</t>
+  </si>
+  <si>
+    <t>PERCENT DIFFERENCE</t>
   </si>
 </sst>
 </file>
@@ -339,7 +330,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +348,14 @@
       <color rgb="FF4A86E8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,11 +387,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15526FD8-3853-4706-ADE8-913345700382}">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -721,9 +721,12 @@
     <col min="8" max="8" width="10.83984375" customWidth="1"/>
     <col min="9" max="9" width="13.734375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.89453125" customWidth="1"/>
+    <col min="12" max="12" width="19.1015625" customWidth="1"/>
+    <col min="13" max="13" width="18.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,188 +746,200 @@
         <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>9.1</v>
+        <v>8.15</v>
       </c>
       <c r="C2">
-        <v>250</v>
+        <v>250.5</v>
       </c>
       <c r="D2" s="2">
         <v>3.931111111111111</v>
       </c>
       <c r="F2">
         <f>D2/(0.05*C2)</f>
-        <v>0.31448888888888887</v>
+        <v>0.31386116655577734</v>
       </c>
       <c r="G2">
         <v>0.31448888888888887</v>
       </c>
       <c r="H2">
         <f>(G2-F2)*100/G2</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
+        <v>0.19960079840318756</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5.15</v>
+      </c>
+      <c r="C3">
+        <v>111</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.6733333333333333</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F33" si="0">D3/(0.05*C3)</f>
+        <v>0.30150150150150146</v>
+      </c>
+      <c r="G3">
+        <v>0.46481481481481463</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H33" si="1">(G3-F3)*100/G3</f>
+        <v>35.135135135135116</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="4">
+        <f>AVERAGE(F2:F33)</f>
+        <v>0.34553416165980361</v>
+      </c>
+      <c r="L3" s="4">
+        <f>AVERAGE(G2:G33)</f>
+        <v>0.38276788001568163</v>
+      </c>
+      <c r="M3">
+        <f>(L3-K3)*100/L3</f>
+        <v>9.7274929010115976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3.55</v>
+      </c>
+      <c r="C4">
+        <v>247.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.1066666666666665</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.25104377104377101</v>
+      </c>
+      <c r="G4">
+        <v>0.18492063492063493</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>-35.757575757575736</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="4">
         <f>MEDIAN(F2:F33)</f>
-        <v>0.26257694866169046</v>
-      </c>
-      <c r="J2">
+        <v>0.3421532576339219</v>
+      </c>
+      <c r="L4" s="4">
         <f>MEDIAN(G2:G33)</f>
         <v>0.36020202020202036</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>5.4</v>
-      </c>
-      <c r="C3">
-        <v>114.5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.6733333333333333</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F33" si="0">D3/(0.05*C3)</f>
-        <v>0.29228529839883549</v>
-      </c>
-      <c r="G3">
-        <v>0.46481481481481463</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H66" si="1">(G3-F3)*100/G3</f>
-        <v>37.117903930130986</v>
-      </c>
-      <c r="I3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C4">
-        <v>340</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.1066666666666665</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0.18274509803921568</v>
-      </c>
-      <c r="G4">
-        <v>0.18492063492063493</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1.1764705882353019</v>
-      </c>
-      <c r="I4">
-        <f>AVERAGE(F2:F33)</f>
-        <v>0.28881830438926193</v>
-      </c>
-      <c r="J4">
-        <f>AVERAGE(G2:G33)</f>
-        <v>0.38276788001568163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4">
+        <f>(L4-K4)*100/L4</f>
+        <v>5.010733298490595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>14.4</v>
       </c>
       <c r="C5">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2">
         <v>1.1022222222222222</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.16090835360908351</v>
+        <v>0.1749559082892416</v>
       </c>
       <c r="G5">
         <v>0.1645107794361525</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>2.1897810218977836</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>-6.3492063492063799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>6.9</v>
+        <v>3.6</v>
       </c>
       <c r="C6">
-        <v>356</v>
+        <v>237</v>
       </c>
       <c r="D6" s="2">
         <v>3.6222222222222222</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.20349563046192259</v>
+        <v>0.30567276136896387</v>
       </c>
       <c r="G6">
         <v>0.30696798493408672</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>33.70786516853935</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.42194092827008151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>6.85</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C7">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D7" s="2">
         <v>1.1599999999999999</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.13892215568862276</v>
+        <v>0.1681159420289855</v>
       </c>
       <c r="G7">
         <v>0.26363636363636372</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>47.305389221556901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>36.231884057971044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -932,221 +947,221 @@
         <v>8.1</v>
       </c>
       <c r="C8">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D8" s="2">
         <v>4.235555555555556</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0.50725216234198278</v>
+        <v>0.51030789825970546</v>
       </c>
       <c r="G8">
         <v>0.51030789825970568</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>0.59880239520960299</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>4.3511888740555699E-14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>8.9</v>
+        <v>8.5</v>
       </c>
       <c r="C9">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2">
         <v>1.6555555555555554</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0.52557319223985877</v>
+        <v>0.54280510018214922</v>
       </c>
       <c r="G9">
         <v>0.55185185185185182</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>4.7619047619047814</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>1.6393442622951004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>6.55</v>
+        <v>6.6</v>
       </c>
       <c r="C10">
-        <v>186.5</v>
+        <v>184</v>
       </c>
       <c r="D10" s="2">
         <v>3.52</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.37747989276139404</v>
+        <v>0.38260869565217387</v>
       </c>
       <c r="G10">
         <v>0.38260869565217381</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>1.3404825737265313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>-1.4508596344533299E-14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>8.9</v>
+        <v>4.3</v>
       </c>
       <c r="C11">
-        <v>227.5</v>
+        <v>181.5</v>
       </c>
       <c r="D11" s="2">
         <v>1.3444444444444446</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.1181929181929182</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="G11">
         <v>0.40740740740740777</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>70.989010989011007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>63.636363636363669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="C12">
-        <v>172</v>
+        <v>169.5</v>
       </c>
       <c r="D12" s="2">
         <v>3.42</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0.39767441860465119</v>
+        <v>0.40353982300884955</v>
       </c>
       <c r="G12">
         <v>0.4071428571428572</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>2.3255813953488427</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.88495575221240352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="C13">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D13" s="2">
         <v>1.2777777777777777</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.22817460317460314</v>
+        <v>0.26345933562428403</v>
       </c>
       <c r="G13">
         <v>0.2839506172839506</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>19.642857142857149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>7.2164948453608355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>6.1</v>
+        <v>3.8</v>
       </c>
       <c r="C14">
-        <v>341.5</v>
+        <v>191</v>
       </c>
       <c r="D14" s="2">
         <v>4.1955555555555559</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0.24571335610867093</v>
+        <v>0.43932518906340895</v>
       </c>
       <c r="G14">
         <v>0.44163742690058483</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>44.363103953147871</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.52356020942409331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>11.8</v>
+        <v>5.6</v>
       </c>
       <c r="C15">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2">
         <v>1.3822222222222222</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.21264957264957265</v>
+        <v>0.31061173533083647</v>
       </c>
       <c r="G15">
         <v>0.31414141414141422</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>32.307692307692321</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>1.123595505617998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="C16">
-        <v>238.5</v>
+        <v>226</v>
       </c>
       <c r="D16" s="2">
         <v>3.88</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0.3253668763102725</v>
+        <v>0.34336283185840705</v>
       </c>
       <c r="G16">
         <v>0.32605042016806723</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>0.20964360587003403</v>
+        <v>-5.3097345132743241</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1154,24 +1169,24 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>6.15</v>
+        <v>6.1</v>
       </c>
       <c r="C17">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2">
         <v>1.2755555555555556</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.180929866036249</v>
+        <v>0.28034188034188035</v>
       </c>
       <c r="G17">
         <v>0.35432098765432085</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>48.936170212765944</v>
+        <v>20.879120879120848</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1179,24 +1194,24 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>17.350000000000001</v>
+        <v>16.45</v>
       </c>
       <c r="C18">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D18" s="2">
         <v>3.068888888888889</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0.33724053724053726</v>
+        <v>0.34481897627965041</v>
       </c>
       <c r="G18">
         <v>0.34098765432098765</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>1.0989010989010921</v>
+        <v>-1.1235955056179705</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1204,24 +1219,24 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>7.95</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>195</v>
+        <v>71.5</v>
       </c>
       <c r="D19" s="2">
         <v>1.3066666666666666</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.13401709401709402</v>
+        <v>0.36550116550116546</v>
       </c>
       <c r="G19">
         <v>0.46666666666666712</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>71.282051282051299</v>
+        <v>21.678321678321762</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1229,24 +1244,24 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="C20">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D20" s="2">
         <v>3.5777777777777779</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0.37075417386298215</v>
+        <v>0.37660818713450295</v>
       </c>
       <c r="G20">
         <v>0.37660818713450295</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>1.5544041450777271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1254,24 +1269,24 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>7.05</v>
+        <v>5.6</v>
       </c>
       <c r="C21">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2">
         <v>1.28</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0.26122448979591834</v>
+        <v>0.26947368421052631</v>
       </c>
       <c r="G21">
         <v>0.27234042553191473</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>4.0816326530611793</v>
+        <v>1.0526315789473117</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1279,24 +1294,24 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="C22">
-        <v>226</v>
+        <v>205.5</v>
       </c>
       <c r="D22" s="2">
         <v>3.7466666666666666</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0.33156342182890852</v>
+        <v>0.36463909164639091</v>
       </c>
       <c r="G22">
         <v>0.33156342182890863</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>3.348448446155943E-14</v>
+        <v>-9.9756690997566633</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1304,24 +1319,24 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>8.8000000000000007</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="C23">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D23" s="2">
         <v>1.2444444444444445</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0.32748538011695905</v>
+        <v>0.34094368340943682</v>
       </c>
       <c r="G23">
         <v>0.34567901234567888</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>5.2631578947368114</v>
+        <v>1.3698630136985985</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1329,24 +1344,24 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>5.95</v>
+        <v>4.2</v>
       </c>
       <c r="C24">
-        <v>308.5</v>
+        <v>219</v>
       </c>
       <c r="D24" s="2">
         <v>4.0711111111111107</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>0.26392940752746258</v>
+        <v>0.37179096905124293</v>
       </c>
       <c r="G24">
         <v>0.37349643221202855</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>29.335494327390617</v>
+        <v>0.45662100456623861</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1354,24 +1369,24 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>6.9</v>
+        <v>5.7</v>
       </c>
       <c r="C25">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D25" s="2">
         <v>1.5266666666666666</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>0.25234159779614324</v>
+        <v>0.29644012944983816</v>
       </c>
       <c r="G25">
         <v>0.37235772357723562</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>32.231404958677665</v>
+        <v>20.388349514563082</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1379,24 +1394,24 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>6.85</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2">
         <v>3.0622222222222222</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>0.59460625674217904</v>
+        <v>0.61244444444444446</v>
       </c>
       <c r="G26">
         <v>0.61244444444444446</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>2.9126213592233086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1404,24 +1419,24 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>9.15</v>
+        <v>4.25</v>
       </c>
       <c r="C27">
-        <v>333</v>
+        <v>99</v>
       </c>
       <c r="D27" s="2">
         <v>1.2</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>7.2072072072072058E-2</v>
+        <v>0.2424242424242424</v>
       </c>
       <c r="G27">
         <v>0.24489795918367352</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>70.570570570570581</v>
+        <v>1.0101010101010388</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1429,24 +1444,24 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>6.35</v>
+        <v>3.8</v>
       </c>
       <c r="C28">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="D28" s="2">
         <v>3.7866666666666666</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>0.3805695142378559</v>
+        <v>0.57373737373737366</v>
       </c>
       <c r="G28">
         <v>0.7573333333333333</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>49.748743718592969</v>
+        <v>24.242424242424249</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1454,24 +1469,24 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>8.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D29" s="2">
         <v>1.3511111111111112</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>0.24565656565656566</v>
+        <v>0.25254413291796468</v>
       </c>
       <c r="G29">
         <v>0.35555555555555585</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>30.909090909090967</v>
+        <v>28.971962616822491</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1479,24 +1494,24 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>7.5</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="C30">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="D30" s="2">
         <v>4.0133333333333336</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>0.25481481481481483</v>
+        <v>0.36484848484848487</v>
       </c>
       <c r="G30">
         <v>0.36484848484848487</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>30.158730158730158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1504,24 +1519,24 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C31">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D31" s="2">
         <v>1.4466666666666668</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>0.22256410256410258</v>
+        <v>0.27820512820512822</v>
       </c>
       <c r="G31">
         <v>0.28933333333333333</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>23.07692307692307</v>
+        <v>3.8461538461538418</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1529,27 +1544,27 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>5.85</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C32">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="D32" s="2">
         <v>3.5933333333333333</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>0.37626527050610814</v>
+        <v>0.46365591397849459</v>
       </c>
       <c r="G32">
         <v>0.46666666666666651</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>19.371727748691086</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.6451612903225532</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1557,1392 +1572,1386 @@
         <v>6.9</v>
       </c>
       <c r="C33">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D33" s="3">
         <v>1.3777777777777778</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>0.40522875816993459</v>
+        <v>0.39935587761674718</v>
       </c>
       <c r="G33">
         <v>0.59903381642512155</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>32.352941176470686</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H35" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H36" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J36" t="s">
-        <v>98</v>
-      </c>
-      <c r="K36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>33.333333333333421</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="C34">
+        <v>308</v>
+      </c>
+      <c r="D34">
+        <v>4.2577777777777781</v>
+      </c>
+      <c r="F34">
+        <f>D34/(0.05*C34)</f>
+        <v>0.27647907647907649</v>
+      </c>
+      <c r="G34">
+        <v>0.27293447293447293</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:H63" si="2">(G34-F34)*100/G34</f>
+        <v>-1.2987012987013058</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>7.7</v>
+      </c>
+      <c r="C35">
+        <v>95</v>
+      </c>
+      <c r="D35">
+        <v>1.0955555555555556</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F86" si="3">D35/(0.05*C35)</f>
+        <v>0.23064327485380118</v>
+      </c>
+      <c r="G35">
+        <v>0.2738888888888889</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>15.789473684210527</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>4.05</v>
+      </c>
+      <c r="C36">
+        <v>281</v>
+      </c>
+      <c r="D36">
+        <v>4.2844444444444445</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0.30494266508501383</v>
+      </c>
+      <c r="G36">
+        <v>0.30386130811662726</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>-0.35587188612099546</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37">
+        <v>6.45</v>
+      </c>
+      <c r="C37">
+        <v>92</v>
+      </c>
+      <c r="D37">
+        <v>1.1155555555555556</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>0.24251207729468599</v>
+      </c>
+      <c r="G37">
+        <v>0.22766439909297059</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>-6.5217391304347494</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" s="4">
+        <f>MEDIAN(F34:F86)</f>
+        <v>0.27985347985347986</v>
+      </c>
+      <c r="K37" s="4">
+        <f>MEDIAN(G34:G86)</f>
+        <v>0.28888888888888892</v>
+      </c>
+      <c r="L37">
+        <f>(K37-J37)*100/K37</f>
+        <v>3.1276415891800586</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>5.45</v>
+      </c>
+      <c r="C38">
+        <v>263</v>
+      </c>
+      <c r="D38">
+        <v>4.08</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0.3102661596958175</v>
+      </c>
+      <c r="G38">
+        <v>0.29142857142857143</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>-6.4638783269962019</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J38" s="4">
+        <f>AVERAGE(F34:F86)</f>
+        <v>0.28209662843670952</v>
+      </c>
+      <c r="K38" s="4">
+        <f>AVERAGE(G34:G86)</f>
+        <v>0.29733392663994251</v>
+      </c>
+      <c r="L38">
+        <f>(K38-J38)*100/K38</f>
+        <v>5.1246416362316607</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>3.6</v>
+      </c>
+      <c r="C39">
+        <v>269.5</v>
+      </c>
+      <c r="D39">
+        <v>3.6155555555555554</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>0.268315811172954</v>
+      </c>
+      <c r="G39">
+        <v>0.26390916463909159</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>-1.6697588126159668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>3.15</v>
+      </c>
+      <c r="C40">
+        <v>148.5</v>
+      </c>
+      <c r="D40">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>0.15622895622895619</v>
+      </c>
+      <c r="G40">
+        <v>0.20350877192982444</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>23.232323232323207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
         <v>4.3</v>
       </c>
-      <c r="C37">
-        <v>314</v>
-      </c>
-      <c r="D37">
-        <v>4.2577777777777781</v>
-      </c>
-      <c r="F37">
-        <f>D37/(0.05*C37)</f>
-        <v>0.27119603680113236</v>
-      </c>
-      <c r="G37">
-        <v>0.27293447293447293</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="1"/>
-        <v>0.63694267515922787</v>
-      </c>
-      <c r="I37" t="s">
-        <v>96</v>
-      </c>
-      <c r="J37">
-        <f>MEDIAN(F37:F89)</f>
-        <v>0.23735224586288417</v>
-      </c>
-      <c r="K37">
-        <f>MEDIAN(G37:G89)</f>
-        <v>0.28888888888888892</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>7.3</v>
-      </c>
-      <c r="C38">
-        <v>98</v>
-      </c>
-      <c r="D38">
-        <v>1.0955555555555556</v>
-      </c>
-      <c r="F38">
-        <f t="shared" ref="F38:F89" si="2">D38/(0.05*C38)</f>
-        <v>0.22358276643990929</v>
-      </c>
-      <c r="G38">
-        <v>0.2738888888888889</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="1"/>
-        <v>18.367346938775515</v>
-      </c>
-      <c r="I38" t="s">
-        <v>97</v>
-      </c>
-      <c r="J38">
-        <f>AVERAGE(F37:F89)</f>
-        <v>0.2255760232134558</v>
-      </c>
-      <c r="K38">
-        <f>AVERAGE(G37:G89)</f>
-        <v>0.29733392663994251</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39">
-        <v>322.5</v>
-      </c>
-      <c r="D39">
-        <v>4.2844444444444445</v>
-      </c>
-      <c r="F39">
+      <c r="C41">
+        <v>185.5</v>
+      </c>
+      <c r="D41">
+        <v>3.9777777777777779</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
+        <v>0.42887091943695715</v>
+      </c>
+      <c r="G41">
+        <v>0.43236714975845397</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="2"/>
-        <v>0.26570198105081827</v>
-      </c>
-      <c r="G39">
-        <v>0.30386130811662726</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="1"/>
-        <v>12.558139534883715</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>6.7</v>
-      </c>
-      <c r="C40">
-        <v>94</v>
-      </c>
-      <c r="D40">
-        <v>1.1155555555555556</v>
-      </c>
-      <c r="F40">
+        <v>0.80862533692719729</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C42">
+        <v>85</v>
+      </c>
+      <c r="D42">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="3"/>
+        <v>0.27294117647058824</v>
+      </c>
+      <c r="G42">
+        <v>0.34117647058823541</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="2"/>
-        <v>0.23735224586288417</v>
-      </c>
-      <c r="G40">
-        <v>0.22766439909297059</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="1"/>
-        <v>-4.2553191489361417</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>6.35</v>
-      </c>
-      <c r="C41">
-        <v>284</v>
-      </c>
-      <c r="D41">
-        <v>4.08</v>
-      </c>
-      <c r="F41">
+        <v>20.000000000000025</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>4.7</v>
+      </c>
+      <c r="C43">
+        <v>150</v>
+      </c>
+      <c r="D43">
+        <v>3.5511111111111111</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="3"/>
+        <v>0.4734814814814815</v>
+      </c>
+      <c r="G43">
+        <v>0.46725146198830403</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="2"/>
-        <v>0.28732394366197184</v>
-      </c>
-      <c r="G41">
-        <v>0.29142857142857143</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="1"/>
-        <v>1.4084507042253491</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C42">
-        <v>358</v>
-      </c>
-      <c r="D42">
-        <v>3.6155555555555554</v>
-      </c>
-      <c r="F42">
+        <v>-1.3333333333333521</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>7.7</v>
+      </c>
+      <c r="C44">
+        <v>69.5</v>
+      </c>
+      <c r="D44">
+        <v>1.2555555555555555</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="3"/>
+        <v>0.3613109512390088</v>
+      </c>
+      <c r="G44">
+        <v>0.35873015873015873</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="2"/>
-        <v>0.20198634388578521</v>
-      </c>
-      <c r="G42">
-        <v>0.26390916463909159</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="1"/>
-        <v>23.463687150837981</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>298</v>
-      </c>
-      <c r="D43">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="F43">
+        <v>-0.71942446043165709</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>4.5</v>
+      </c>
+      <c r="C45">
+        <v>223</v>
+      </c>
+      <c r="D45">
+        <v>4.1422222222222222</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>0.3714997508719482</v>
+      </c>
+      <c r="G45">
+        <v>0.36019323671497583</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="2"/>
-        <v>7.7852348993288578E-2</v>
-      </c>
-      <c r="G43">
-        <v>0.20350877192982444</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="1"/>
-        <v>61.744966442953007</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C44">
-        <v>291</v>
-      </c>
-      <c r="D44">
-        <v>3.9777777777777779</v>
-      </c>
-      <c r="F44">
+        <v>-3.1390134529148077</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>9.6</v>
+      </c>
+      <c r="C46">
+        <v>84</v>
+      </c>
+      <c r="D46">
+        <v>1.1933333333333334</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="3"/>
+        <v>0.28412698412698412</v>
+      </c>
+      <c r="G46">
+        <v>0.28412698412698395</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="2"/>
-        <v>0.27338678885070639</v>
-      </c>
-      <c r="G44">
-        <v>0.43236714975845397</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="1"/>
-        <v>36.769759450171804</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C45">
-        <v>86</v>
-      </c>
-      <c r="D45">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="F45">
+        <v>-5.8612332864289032E-14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C47">
+        <v>193</v>
+      </c>
+      <c r="D47">
+        <v>4.1577777777777776</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>0.43085780080598729</v>
+      </c>
+      <c r="G47">
+        <v>0.42426303854875291</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="2"/>
-        <v>0.26976744186046508</v>
-      </c>
-      <c r="G45">
-        <v>0.34117647058823541</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="1"/>
-        <v>20.930232558139572</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>3.4</v>
-      </c>
-      <c r="C46">
-        <v>183</v>
-      </c>
-      <c r="D46">
-        <v>3.5511111111111111</v>
-      </c>
-      <c r="F46">
+        <v>-1.5544041450776909</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>6.4</v>
+      </c>
+      <c r="C48">
+        <v>65</v>
+      </c>
+      <c r="D48">
+        <v>1.3866666666666667</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>0.42666666666666669</v>
+      </c>
+      <c r="G48">
+        <v>0.43333333333333296</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="2"/>
-        <v>0.38809957498482089</v>
-      </c>
-      <c r="G46">
-        <v>0.46725146198830403</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="1"/>
-        <v>16.9398907103825</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47">
-        <v>7.8</v>
-      </c>
-      <c r="C47">
-        <v>72</v>
-      </c>
-      <c r="D47">
-        <v>1.2555555555555555</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="2"/>
-        <v>0.34876543209876543</v>
-      </c>
-      <c r="G47">
-        <v>0.35873015873015873</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="1"/>
-        <v>2.7777777777777799</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="C48">
-        <v>240</v>
-      </c>
-      <c r="D48">
-        <v>4.1422222222222222</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="2"/>
-        <v>0.34518518518518521</v>
-      </c>
-      <c r="G48">
-        <v>0.36019323671497583</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="1"/>
-        <v>4.1666666666666563</v>
+        <v>1.5384615384614473</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49">
-        <v>9.1999999999999993</v>
+        <v>3.45</v>
       </c>
       <c r="C49">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="D49">
-        <v>1.1933333333333334</v>
+        <v>4.0866666666666669</v>
       </c>
       <c r="F49">
+        <f t="shared" si="3"/>
+        <v>0.32052287581699346</v>
+      </c>
+      <c r="G49">
+        <v>0.40065359477124174</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="2"/>
-        <v>0.27751937984496128</v>
-      </c>
-      <c r="G49">
-        <v>0.28412698412698395</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="1"/>
-        <v>2.3255813953487632</v>
+        <v>19.999999999999982</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50">
-        <v>8.3000000000000007</v>
+        <v>5.6</v>
       </c>
       <c r="C50">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="D50">
-        <v>4.1577777777777776</v>
+        <v>1.4488888888888889</v>
       </c>
       <c r="F50">
+        <f t="shared" si="3"/>
+        <v>0.18340365682137832</v>
+      </c>
+      <c r="G50">
+        <v>0.17887517146776402</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="2"/>
-        <v>0.4242630385487528</v>
-      </c>
-      <c r="G50">
-        <v>0.42426303854875291</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="1"/>
-        <v>2.6168271184377016E-14</v>
+        <v>-2.5316455696202667</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>6.4</v>
+        <v>3.3</v>
       </c>
       <c r="C51">
-        <v>68</v>
+        <v>283</v>
       </c>
       <c r="D51">
-        <v>1.3866666666666667</v>
+        <v>4.12</v>
       </c>
       <c r="F51">
+        <f t="shared" si="3"/>
+        <v>0.29116607773851588</v>
+      </c>
+      <c r="G51">
+        <v>0.29219858156028367</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="2"/>
-        <v>0.40784313725490196</v>
-      </c>
-      <c r="G51">
-        <v>0.43333333333333296</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="1"/>
-        <v>5.8823529411763911</v>
+        <v>0.35335689045936264</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
-        <v>4.2</v>
+        <v>8.35</v>
       </c>
       <c r="C52">
-        <v>351</v>
+        <v>126</v>
       </c>
       <c r="D52">
-        <v>4.0866666666666669</v>
+        <v>1.7066666666666668</v>
       </c>
       <c r="F52">
+        <f t="shared" si="3"/>
+        <v>0.27089947089947086</v>
+      </c>
+      <c r="G52">
+        <v>0.27978142076502727</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="2"/>
-        <v>0.23285849952516618</v>
-      </c>
-      <c r="G52">
-        <v>0.40065359477124174</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="1"/>
-        <v>41.880341880341867</v>
+        <v>3.1746031746031687</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>5.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C53">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D53">
-        <v>1.4488888888888889</v>
+        <v>3.7111111111111112</v>
       </c>
       <c r="F53">
+        <f t="shared" si="3"/>
+        <v>0.42656449553001274</v>
+      </c>
+      <c r="G53">
+        <v>0.31450094161958575</v>
+      </c>
+      <c r="H53">
         <f t="shared" si="2"/>
-        <v>0.17562289562289563</v>
-      </c>
-      <c r="G53">
-        <v>0.17887517146776402</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="1"/>
-        <v>1.8181818181817957</v>
+        <v>-35.632183908045938</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
-        <v>4.8</v>
+        <v>19.8</v>
       </c>
       <c r="C54">
-        <v>785.5</v>
+        <v>75</v>
       </c>
       <c r="D54">
-        <v>4.12</v>
+        <v>1.0777777777777777</v>
       </c>
       <c r="F54">
+        <f t="shared" si="3"/>
+        <v>0.28740740740740739</v>
+      </c>
+      <c r="G54">
+        <v>0.29129129129129105</v>
+      </c>
+      <c r="H54">
         <f t="shared" si="2"/>
-        <v>0.10490133672819858</v>
-      </c>
-      <c r="G54">
-        <v>0.29219858156028367</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="1"/>
-        <v>64.09929980903884</v>
+        <v>1.3333333333332593</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>8.4499999999999993</v>
+        <v>5.7</v>
       </c>
       <c r="C55">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="D55">
-        <v>1.7066666666666668</v>
+        <v>3.5466666666666669</v>
       </c>
       <c r="F55">
+        <f t="shared" si="3"/>
+        <v>0.3511551155115511</v>
+      </c>
+      <c r="G55">
+        <v>0.29803921568627456</v>
+      </c>
+      <c r="H55">
         <f t="shared" si="2"/>
-        <v>0.26876640419947506</v>
-      </c>
-      <c r="G55">
-        <v>0.27978142076502727</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="1"/>
-        <v>3.9370078740157304</v>
+        <v>-17.821782178217781</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>10.5</v>
+        <v>6.85</v>
       </c>
       <c r="C56">
-        <v>239</v>
+        <v>83</v>
       </c>
       <c r="D56">
-        <v>3.7111111111111112</v>
+        <v>1.0644444444444445</v>
       </c>
       <c r="F56">
+        <f t="shared" si="3"/>
+        <v>0.25649263721552878</v>
+      </c>
+      <c r="G56">
+        <v>0.26611111111111113</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="2"/>
-        <v>0.31055323105532306</v>
-      </c>
-      <c r="G56">
-        <v>0.31450094161958575</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="1"/>
-        <v>1.2552301255230451</v>
+        <v>3.6144578313253075</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>19.8</v>
+        <v>3.45</v>
       </c>
       <c r="C57">
-        <v>76</v>
+        <v>299.5</v>
       </c>
       <c r="D57">
-        <v>1.0777777777777777</v>
+        <v>4.24</v>
       </c>
       <c r="F57">
+        <f t="shared" si="3"/>
+        <v>0.28313856427378964</v>
+      </c>
+      <c r="G57">
+        <v>0.28648648648648656</v>
+      </c>
+      <c r="H57">
         <f t="shared" si="2"/>
-        <v>0.283625730994152</v>
-      </c>
-      <c r="G57">
-        <v>0.29129129129129105</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="1"/>
-        <v>2.6315789473683568</v>
+        <v>1.1686143572621317</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>6.7</v>
+        <v>4.7</v>
       </c>
       <c r="C58">
-        <v>241</v>
+        <v>128</v>
       </c>
       <c r="D58">
-        <v>3.5466666666666669</v>
+        <v>1.52</v>
       </c>
       <c r="F58">
+        <f t="shared" si="3"/>
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="G58">
+        <v>0.24516129032258052</v>
+      </c>
+      <c r="H58">
         <f t="shared" si="2"/>
-        <v>0.29432918395573998</v>
-      </c>
-      <c r="G58">
-        <v>0.29803921568627456</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="1"/>
-        <v>1.2448132780083128</v>
+        <v>3.1249999999999556</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>6.8</v>
+        <v>3.5</v>
       </c>
       <c r="C59">
-        <v>105.5</v>
+        <v>273</v>
       </c>
       <c r="D59">
-        <v>1.0644444444444445</v>
+        <v>3.82</v>
       </c>
       <c r="F59">
+        <f t="shared" si="3"/>
+        <v>0.27985347985347986</v>
+      </c>
+      <c r="G59">
+        <v>0.28296296296296297</v>
+      </c>
+      <c r="H59">
         <f t="shared" si="2"/>
-        <v>0.20179041600842548</v>
-      </c>
-      <c r="G59">
-        <v>0.26611111111111113</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="1"/>
-        <v>24.170616113744082</v>
+        <v>1.0989010989011001</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60">
-        <v>4.6500000000000004</v>
+        <v>7.1</v>
       </c>
       <c r="C60">
-        <v>341</v>
+        <v>122</v>
       </c>
       <c r="D60">
-        <v>4.24</v>
+        <v>1.4</v>
       </c>
       <c r="F60">
+        <f t="shared" si="3"/>
+        <v>0.22950819672131145</v>
+      </c>
+      <c r="G60">
+        <v>0.23333333333333331</v>
+      </c>
+      <c r="H60">
         <f t="shared" si="2"/>
-        <v>0.24868035190615836</v>
-      </c>
-      <c r="G60">
-        <v>0.28648648648648656</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="1"/>
-        <v>13.196480938416443</v>
+        <v>1.6393442622950816</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B61">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="C61">
-        <v>129</v>
+        <v>285</v>
       </c>
       <c r="D61">
-        <v>1.52</v>
+        <v>4.2733333333333334</v>
       </c>
       <c r="F61">
+        <f t="shared" si="3"/>
+        <v>0.29988304093567253</v>
+      </c>
+      <c r="G61">
+        <v>0.33126614987080105</v>
+      </c>
+      <c r="H61">
         <f t="shared" si="2"/>
-        <v>0.23565891472868217</v>
-      </c>
-      <c r="G61">
-        <v>0.24516129032258052</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="1"/>
-        <v>3.8759689922480152</v>
+        <v>9.4736842105263168</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B62">
-        <v>3.3</v>
+        <v>8.6</v>
       </c>
       <c r="C62">
-        <v>282</v>
+        <v>82</v>
       </c>
       <c r="D62">
-        <v>3.82</v>
+        <v>1.4044444444444444</v>
       </c>
       <c r="F62">
+        <f t="shared" si="3"/>
+        <v>0.34254742547425471</v>
+      </c>
+      <c r="G62">
+        <v>0.33439153439153413</v>
+      </c>
+      <c r="H62">
         <f t="shared" si="2"/>
-        <v>0.27092198581560278</v>
-      </c>
-      <c r="G62">
-        <v>0.28296296296296297</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="1"/>
-        <v>4.2553191489361923</v>
+        <v>-2.4390243902439726</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B63">
-        <v>7.1</v>
+        <v>3.1</v>
       </c>
       <c r="C63">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="D63">
-        <v>1.4</v>
+        <v>3.7422222222222223</v>
       </c>
       <c r="F63">
+        <f t="shared" si="3"/>
+        <v>0.38579610538373421</v>
+      </c>
+      <c r="G63">
+        <v>0.38185941043083915</v>
+      </c>
+      <c r="H63">
         <f t="shared" si="2"/>
-        <v>0.22580645161290319</v>
-      </c>
-      <c r="G63">
-        <v>0.23333333333333331</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="1"/>
-        <v>3.2258064516129079</v>
+        <v>-1.0309278350514965</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B64">
-        <v>4.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C64">
-        <v>289.5</v>
+        <v>88</v>
       </c>
       <c r="D64">
-        <v>4.2733333333333334</v>
+        <v>1.38</v>
       </c>
       <c r="F64">
-        <f t="shared" si="2"/>
-        <v>0.29522164651698329</v>
+        <f t="shared" si="3"/>
+        <v>0.3136363636363636</v>
       </c>
       <c r="G64">
-        <v>0.33126614987080105</v>
+        <v>0.32093023255813974</v>
       </c>
       <c r="H64">
-        <f t="shared" si="1"/>
-        <v>10.88082901554405</v>
+        <f t="shared" ref="H64:H86" si="4">(G64-F64)*100/G64</f>
+        <v>2.2727272727273453</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>4.3</v>
       </c>
       <c r="C65">
-        <v>82</v>
+        <v>284</v>
       </c>
       <c r="D65">
-        <v>1.4044444444444444</v>
+        <v>3.7044444444444444</v>
       </c>
       <c r="F65">
-        <f t="shared" si="2"/>
-        <v>0.34254742547425471</v>
+        <f t="shared" si="3"/>
+        <v>0.26087636932707353</v>
       </c>
       <c r="G65">
-        <v>0.33439153439153413</v>
+        <v>0.25725308641975309</v>
       </c>
       <c r="H65">
-        <f t="shared" si="1"/>
-        <v>-2.4390243902439726</v>
+        <f t="shared" si="4"/>
+        <v>-1.4084507042253445</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B66">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="C66">
-        <v>387</v>
+        <v>103</v>
       </c>
       <c r="D66">
-        <v>3.7422222222222223</v>
+        <v>1.1288888888888888</v>
       </c>
       <c r="F66">
-        <f t="shared" si="2"/>
-        <v>0.19339649727246624</v>
+        <f t="shared" si="3"/>
+        <v>0.21920172599784249</v>
       </c>
       <c r="G66">
-        <v>0.38185941043083915</v>
+        <v>0.25656565656565661</v>
       </c>
       <c r="H66">
-        <f t="shared" si="1"/>
-        <v>49.354005167958682</v>
+        <f t="shared" si="4"/>
+        <v>14.563106796116525</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B67">
-        <v>5.5</v>
+        <v>3.55</v>
       </c>
       <c r="C67">
-        <v>127.5</v>
+        <v>327</v>
       </c>
       <c r="D67">
-        <v>1.38</v>
+        <v>1.2288888888888889</v>
       </c>
       <c r="F67">
-        <f t="shared" si="2"/>
-        <v>0.21647058823529411</v>
+        <f t="shared" si="3"/>
+        <v>7.5161399932042128E-2</v>
       </c>
       <c r="G67">
-        <v>0.32093023255813974</v>
+        <v>0.24577777777777779</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H89" si="3">(G67-F67)*100/G67</f>
-        <v>32.549019607843185</v>
+        <f t="shared" si="4"/>
+        <v>69.418960244648318</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B68">
-        <v>4.8</v>
+        <v>3.6</v>
       </c>
       <c r="C68">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="D68">
-        <v>3.7044444444444444</v>
+        <v>4.5733333333333333</v>
       </c>
       <c r="F68">
-        <f t="shared" si="2"/>
-        <v>0.2494575383464272</v>
+        <f t="shared" si="3"/>
+        <v>0.34910941475826968</v>
       </c>
       <c r="G68">
-        <v>0.25725308641975309</v>
+        <v>0.47147766323024043</v>
       </c>
       <c r="H68">
-        <f t="shared" si="3"/>
-        <v>3.030303030303044</v>
+        <f t="shared" si="4"/>
+        <v>25.954198473282435</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B69">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="C69">
-        <v>283</v>
+        <v>106</v>
       </c>
       <c r="D69">
-        <v>1.1288888888888888</v>
+        <v>1.2622222222222221</v>
       </c>
       <c r="F69">
-        <f t="shared" si="2"/>
-        <v>7.9780133490380836E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.23815513626834375</v>
       </c>
       <c r="G69">
-        <v>0.25656565656565661</v>
+        <v>0.23815513626834392</v>
       </c>
       <c r="H69">
-        <f t="shared" si="3"/>
-        <v>68.904593639575978</v>
+        <f t="shared" si="4"/>
+        <v>6.9926458989374926E-14</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>4.3</v>
+        <v>3.2</v>
       </c>
       <c r="C70">
-        <v>407</v>
+        <v>300</v>
       </c>
       <c r="D70">
-        <v>1.2288888888888889</v>
+        <v>4.6977777777777776</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
-        <v>6.0387660387660386E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.31318518518518518</v>
       </c>
       <c r="G70">
-        <v>0.24577777777777779</v>
+        <v>0.31528709917971665</v>
       </c>
       <c r="H70">
-        <f t="shared" si="3"/>
-        <v>75.429975429975428</v>
+        <f t="shared" si="4"/>
+        <v>0.66666666666667418</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C71">
-        <v>455</v>
+        <v>255.5</v>
       </c>
       <c r="D71">
-        <v>4.5733333333333333</v>
+        <v>3.9155555555555557</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
-        <v>0.20102564102564102</v>
+        <f t="shared" si="3"/>
+        <v>0.30650141335072845</v>
       </c>
       <c r="G71">
-        <v>0.47147766323024043</v>
+        <v>0.3375478927203065</v>
       </c>
       <c r="H71">
-        <f t="shared" si="3"/>
-        <v>57.362637362637358</v>
+        <f t="shared" si="4"/>
+        <v>9.1976516634050753</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B72">
-        <v>4.55</v>
+        <v>3.1</v>
       </c>
       <c r="C72">
-        <v>331</v>
+        <v>121</v>
       </c>
       <c r="D72">
-        <v>1.2622222222222221</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="F72">
-        <f t="shared" si="2"/>
-        <v>7.6267203759650876E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.15977961432506885</v>
       </c>
       <c r="G72">
-        <v>0.23815513626834392</v>
+        <v>0.21014492753623182</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
-        <v>67.975830815709983</v>
+        <f t="shared" si="4"/>
+        <v>23.966942148760317</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B73">
-        <v>3.85</v>
+        <v>2.8</v>
       </c>
       <c r="C73">
-        <v>330.5</v>
+        <v>334</v>
       </c>
       <c r="D73">
-        <v>4.6977777777777776</v>
+        <v>4.4444444444444446</v>
       </c>
       <c r="F73">
-        <f t="shared" si="2"/>
-        <v>0.28428307278534204</v>
+        <f t="shared" si="3"/>
+        <v>0.26613439787092485</v>
       </c>
       <c r="G73">
-        <v>0.31528709917971665</v>
+        <v>0.22792022792022792</v>
       </c>
       <c r="H73">
-        <f t="shared" si="3"/>
-        <v>9.8335854765506969</v>
+        <f t="shared" si="4"/>
+        <v>-16.766467065868277</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="C74">
-        <v>327</v>
+        <v>174</v>
       </c>
       <c r="D74">
-        <v>3.9155555555555557</v>
+        <v>1.3111111111111111</v>
       </c>
       <c r="F74">
-        <f t="shared" si="2"/>
-        <v>0.23948352021746516</v>
+        <f t="shared" si="3"/>
+        <v>0.15070242656449551</v>
       </c>
       <c r="G74">
-        <v>0.3375478927203065</v>
+        <v>0.29135802469135802</v>
       </c>
       <c r="H74">
-        <f t="shared" si="3"/>
-        <v>29.051987767584098</v>
+        <f t="shared" si="4"/>
+        <v>48.275862068965523</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B75">
-        <v>2.15</v>
+        <v>3.65</v>
       </c>
       <c r="C75">
-        <v>126</v>
+        <v>235.5</v>
       </c>
       <c r="D75">
-        <v>0.96666666666666667</v>
+        <v>3.7155555555555555</v>
       </c>
       <c r="F75">
-        <f t="shared" si="2"/>
-        <v>0.15343915343915343</v>
+        <f t="shared" si="3"/>
+        <v>0.31554611936777538</v>
       </c>
       <c r="G75">
-        <v>0.21014492753623182</v>
+        <v>0.31756885090218417</v>
       </c>
       <c r="H75">
-        <f t="shared" si="3"/>
-        <v>26.984126984126966</v>
+        <f t="shared" si="4"/>
+        <v>0.63694267515922887</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B76">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="C76">
-        <v>393</v>
+        <v>135.5</v>
       </c>
       <c r="D76">
-        <v>4.4444444444444446</v>
+        <v>1.2066666666666668</v>
       </c>
       <c r="F76">
-        <f t="shared" si="2"/>
-        <v>0.22618037885213457</v>
+        <f t="shared" si="3"/>
+        <v>0.17810578105781058</v>
       </c>
       <c r="G76">
-        <v>0.22792022792022792</v>
+        <v>0.18282828282828281</v>
       </c>
       <c r="H76">
-        <f t="shared" si="3"/>
-        <v>0.76335877862595825</v>
+        <f t="shared" si="4"/>
+        <v>2.5830258302582925</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B77">
-        <v>5.05</v>
+        <v>2.9</v>
       </c>
       <c r="C77">
-        <v>432.5</v>
+        <v>260</v>
       </c>
       <c r="D77">
-        <v>1.3111111111111111</v>
+        <v>3.7266666666666666</v>
       </c>
       <c r="F77">
-        <f t="shared" si="2"/>
-        <v>6.0629415542710341E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.28666666666666668</v>
       </c>
       <c r="G77">
-        <v>0.29135802469135802</v>
+        <v>0.28888888888888892</v>
       </c>
       <c r="H77">
-        <f t="shared" si="3"/>
-        <v>79.190751445086704</v>
+        <f t="shared" si="4"/>
+        <v>0.76923076923077416</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>3.8</v>
       </c>
       <c r="C78">
-        <v>284</v>
+        <v>142</v>
       </c>
       <c r="D78">
-        <v>3.7155555555555555</v>
+        <v>1.048888888888889</v>
       </c>
       <c r="F78">
-        <f t="shared" si="2"/>
-        <v>0.26165884194053207</v>
+        <f t="shared" si="3"/>
+        <v>0.14773082942097027</v>
       </c>
       <c r="G78">
-        <v>0.31756885090218417</v>
+        <v>0.24973544973544959</v>
       </c>
       <c r="H78">
-        <f t="shared" si="3"/>
-        <v>17.605633802816889</v>
+        <f t="shared" si="4"/>
+        <v>40.845070422535173</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B79">
-        <v>14.3</v>
+        <v>3.5</v>
       </c>
       <c r="C79">
-        <v>586</v>
+        <v>174</v>
       </c>
       <c r="D79">
-        <v>1.2066666666666668</v>
+        <v>3.5333333333333332</v>
       </c>
       <c r="F79">
-        <f t="shared" si="2"/>
-        <v>4.1183162684869171E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.40613026819923365</v>
       </c>
       <c r="G79">
-        <v>0.18282828282828281</v>
+        <v>0.41085271317829447</v>
       </c>
       <c r="H79">
-        <f t="shared" si="3"/>
-        <v>77.474402730375417</v>
+        <f t="shared" si="4"/>
+        <v>1.1494252873563142</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B80">
-        <v>2.75</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>393.5</v>
+        <v>113</v>
       </c>
       <c r="D80">
-        <v>3.7266666666666666</v>
+        <v>1.22</v>
       </c>
       <c r="F80">
-        <f t="shared" si="2"/>
-        <v>0.18941126641253705</v>
+        <f t="shared" si="3"/>
+        <v>0.21592920353982298</v>
       </c>
       <c r="G80">
-        <v>0.28888888888888892</v>
+        <v>0.21403508771929813</v>
       </c>
       <c r="H80">
-        <f t="shared" si="3"/>
-        <v>34.434561626429485</v>
+        <f t="shared" si="4"/>
+        <v>-0.88495575221242773</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B81">
-        <v>10.9</v>
+        <v>2.8</v>
       </c>
       <c r="C81">
-        <v>636.5</v>
+        <v>261</v>
       </c>
       <c r="D81">
-        <v>1.048888888888889</v>
+        <v>3.34</v>
       </c>
       <c r="F81">
-        <f t="shared" si="2"/>
-        <v>3.2958016932879461E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.25593869731800761</v>
       </c>
       <c r="G81">
-        <v>0.24973544973544959</v>
+        <v>0.25692307692307692</v>
       </c>
       <c r="H81">
-        <f t="shared" si="3"/>
-        <v>86.802827965435966</v>
+        <f t="shared" si="4"/>
+        <v>0.38314176245212572</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>5.7</v>
+        <v>3.7</v>
       </c>
       <c r="C82">
-        <v>436</v>
+        <v>132.5</v>
       </c>
       <c r="D82">
-        <v>3.5333333333333332</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
-        <v>0.1620795107033639</v>
+        <f t="shared" si="3"/>
+        <v>0.17509433962264151</v>
       </c>
       <c r="G82">
-        <v>0.41085271317829447</v>
+        <v>0.17846153846153845</v>
       </c>
       <c r="H82">
-        <f t="shared" si="3"/>
-        <v>60.550458715596321</v>
+        <f t="shared" si="4"/>
+        <v>1.8867924528301818</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B83">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="C83">
-        <v>116</v>
+        <v>319</v>
       </c>
       <c r="D83">
-        <v>1.22</v>
+        <v>4.0777777777777775</v>
       </c>
       <c r="F83">
-        <f t="shared" si="2"/>
-        <v>0.21034482758620687</v>
+        <f t="shared" si="3"/>
+        <v>0.25566004876349702</v>
       </c>
       <c r="G83">
-        <v>0.21403508771929813</v>
+        <v>0.24417831004657345</v>
       </c>
       <c r="H83">
-        <f t="shared" si="3"/>
-        <v>1.7241379310344425</v>
+        <f t="shared" si="4"/>
+        <v>-4.7021943573667926</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B84">
-        <v>3.15</v>
+        <v>4.25</v>
       </c>
       <c r="C84">
-        <v>370</v>
+        <v>126</v>
       </c>
       <c r="D84">
-        <v>3.34</v>
+        <v>1.3133333333333332</v>
       </c>
       <c r="F84">
-        <f t="shared" si="2"/>
-        <v>0.18054054054054053</v>
+        <f t="shared" si="3"/>
+        <v>0.20846560846560844</v>
       </c>
       <c r="G84">
-        <v>0.25692307692307692</v>
+        <v>0.29848484848484858</v>
       </c>
       <c r="H84">
-        <f t="shared" si="3"/>
-        <v>29.729729729729733</v>
+        <f t="shared" si="4"/>
+        <v>30.15873015873019</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B85">
-        <v>6.3</v>
+        <v>5</v>
       </c>
       <c r="C85">
-        <v>475</v>
+        <v>273</v>
       </c>
       <c r="D85">
-        <v>1.1599999999999999</v>
+        <v>4.3177777777777777</v>
       </c>
       <c r="F85">
-        <f t="shared" si="2"/>
-        <v>4.8842105263157888E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.31632071632071629</v>
       </c>
       <c r="G85">
-        <v>0.17846153846153845</v>
+        <v>0.31288244766505641</v>
       </c>
       <c r="H85">
-        <f t="shared" si="3"/>
-        <v>72.631578947368425</v>
+        <f t="shared" si="4"/>
+        <v>-1.0989010989010737</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B86">
-        <v>4.5</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="C86">
-        <v>337</v>
+        <v>116</v>
       </c>
       <c r="D86">
-        <v>4.0777777777777775</v>
+        <v>1.4622222222222223</v>
       </c>
       <c r="F86">
-        <f t="shared" si="2"/>
-        <v>0.24200461589185621</v>
+        <f t="shared" si="3"/>
+        <v>0.25210727969348656</v>
       </c>
       <c r="G86">
-        <v>0.24417831004657345</v>
+        <v>0.27589098532494777</v>
       </c>
       <c r="H86">
-        <f t="shared" si="3"/>
-        <v>0.89020771513351959</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87">
-        <v>4.45</v>
-      </c>
-      <c r="C87">
-        <v>128</v>
-      </c>
-      <c r="D87">
-        <v>1.3133333333333332</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="2"/>
-        <v>0.2052083333333333</v>
-      </c>
-      <c r="G87">
-        <v>0.29848484848484858</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="3"/>
-        <v>31.250000000000032</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <v>7.05</v>
-      </c>
-      <c r="C88">
-        <v>282.5</v>
-      </c>
-      <c r="D88">
-        <v>4.3177777777777777</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="2"/>
-        <v>0.30568338249754179</v>
-      </c>
-      <c r="G88">
-        <v>0.31288244766505641</v>
-      </c>
-      <c r="H88">
-        <f t="shared" si="3"/>
-        <v>2.3008849557522271</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89">
-        <v>4.3</v>
-      </c>
-      <c r="C89">
-        <v>120</v>
-      </c>
-      <c r="D89">
-        <v>1.4622222222222223</v>
-      </c>
-      <c r="F89">
-        <f t="shared" si="2"/>
-        <v>0.24370370370370373</v>
-      </c>
-      <c r="G89">
-        <v>0.27589098532494777</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="3"/>
-        <v>11.666666666666716</v>
+        <f t="shared" si="4"/>
+        <v>8.6206896551724821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>